<commit_message>
Partial update to Gabor lens in BeamLineElement
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/GaborLens.xlsx
+++ b/21-Spreads4Tests/GaborLens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75ED890-372F-D547-9761-A7E79E05A00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16619366-3F9E-FB4A-A9B7-F2C75E64207E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="640" windowWidth="23260" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>MeV</t>
   </si>
@@ -272,9 +272,6 @@
     <t>J-MeV relationship</t>
   </si>
   <si>
-    <t>1/m</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
   </si>
   <si>
     <t>Natural units</t>
-  </si>
-  <si>
-    <t>B/l element</t>
   </si>
   <si>
     <r>
@@ -317,20 +311,6 @@
   </si>
   <si>
     <r>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>-0.5</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>sin(</t>
     </r>
     <r>
@@ -416,7 +396,7 @@
   </si>
   <si>
     <r>
-      <t>m</t>
+      <t>m-(MeV</t>
     </r>
     <r>
       <rPr>
@@ -436,17 +416,114 @@
         <family val="2"/>
         <charset val="2"/>
       </rPr>
-      <t>-(MeV</t>
+      <t>) relationship</t>
+    </r>
+  </si>
+  <si>
+    <t>h(bar)c</t>
+  </si>
+  <si>
+    <t>MeV fm</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <r>
+      <t>MeV</t>
     </r>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <rFont val="Calibri (Body)"/>
       </rPr>
       <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>z</t>
+    </r>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>e</t>
     </r>
     <r>
       <rPr>
@@ -454,25 +531,81 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>) relationship</t>
-    </r>
-  </si>
-  <si>
-    <t>h(bar)c</t>
-  </si>
-  <si>
-    <t>MeV fm</t>
-  </si>
-  <si>
-    <t>fm</t>
-  </si>
-  <si>
-    <t>MeV-1</t>
-  </si>
-  <si>
-    <t>cm</t>
+      <t>(trans)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(longi)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <t>B/l element i/p parameters</t>
   </si>
 </sst>
 </file>
@@ -482,7 +615,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -962,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -988,7 +1121,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1003,7 +1135,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1033,6 +1164,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,12 +1195,9 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1084,18 +1234,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,8 +1256,8 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:colOff>319616</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>16510</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1907638" cy="392608"/>
@@ -1138,7 +1276,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8947150" y="969010"/>
+              <a:off x="9218083" y="2624243"/>
               <a:ext cx="1907638" cy="392608"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1484,7 +1622,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8947150" y="969010"/>
+              <a:off x="9218083" y="2624243"/>
               <a:ext cx="1907638" cy="392608"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1574,9 +1712,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>402590</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>54610</xdr:rowOff>
+      <xdr:colOff>309457</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>20744</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2865272" cy="378245"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -1594,7 +1732,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8936990" y="1464310"/>
+              <a:off x="9207924" y="3060277"/>
               <a:ext cx="2865272" cy="378245"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2034,7 +2172,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8936990" y="1464310"/>
+              <a:off x="9207924" y="3060277"/>
               <a:ext cx="2865272" cy="378245"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2167,6 +2305,1328 @@
                 <a:t>(J–MeV relationship)</a:t>
               </a:r>
               <a:endParaRPr lang="en-GB" sz="1100" i="0"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>284057</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33444</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3207545" cy="378245"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6EFE474-AF12-D345-84EE-32449BDA93BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9182524" y="3504777"/>
+              <a:ext cx="3207545" cy="378245"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑘</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑍</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑒</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜀</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝛾</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝑟</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝒎</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝒑</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:d>
+                          <m:dPr>
+                            <m:begChr m:val="["/>
+                            <m:endChr m:val="]"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="0">
+                                <a:solidFill>
+                                  <a:schemeClr val="tx1"/>
+                                </a:solidFill>
+                                <a:effectLst/>
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="+mn-ea"/>
+                                <a:cs typeface="+mn-cs"/>
+                              </a:rPr>
+                              <m:t>𝐌𝐞𝐕</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:d>
+                      </m:num>
+                      <m:den>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝒑</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝒓</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝟐</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                        <m:d>
+                          <m:dPr>
+                            <m:begChr m:val="["/>
+                            <m:endChr m:val="]"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                    <a:solidFill>
+                                      <a:schemeClr val="tx1"/>
+                                    </a:solidFill>
+                                    <a:effectLst/>
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    <a:ea typeface="+mn-ea"/>
+                                    <a:cs typeface="+mn-cs"/>
+                                  </a:rPr>
+                                  <m:t>𝑴𝒆𝑽</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="en-GB" sz="1100" b="1" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝟐</m:t>
+                                </m:r>
+                              </m:sup>
+                            </m:sSup>
+                          </m:e>
+                        </m:d>
+                      </m:den>
+                    </m:f>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>/</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>(</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>m</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <m:rPr>
+                            <m:nor/>
+                          </m:rPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>MeV</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>relationship</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100" i="0"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6EFE474-AF12-D345-84EE-32449BDA93BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9182524" y="3504777"/>
+              <a:ext cx="3207545" cy="378245"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑘=(𝑍𝑒^2)/(2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜀_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0 ) </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> (𝛾_𝑟</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 𝒎_𝒑 [𝐌𝐞𝐕]</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>)/(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝒑_𝒓^𝟐 [〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑴𝒆𝑽〗^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝟐 ]</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> ) 𝑛_𝑒</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(m−〖"MeV" 〗^(−1)) relationship)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100" i="0"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>643466</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1758815" cy="502958"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCF1D1E4-28D9-C2D7-1FB8-2754356A24DB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10490199" y="785284"/>
+              <a:ext cx="1758815" cy="502958"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>longi</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>4</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜖</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑉</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐴</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑅</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑝</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1+2</m:t>
+                            </m:r>
+                            <m:func>
+                              <m:funcPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:funcPr>
+                              <m:fName>
+                                <m:r>
+                                  <m:rPr>
+                                    <m:sty m:val="p"/>
+                                  </m:rPr>
+                                  <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>ln</m:t>
+                                </m:r>
+                              </m:fName>
+                              <m:e>
+                                <m:d>
+                                  <m:dPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:dPr>
+                                  <m:e>
+                                    <m:f>
+                                      <m:fPr>
+                                        <m:ctrlPr>
+                                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                        </m:ctrlPr>
+                                      </m:fPr>
+                                      <m:num>
+                                        <m:sSub>
+                                          <m:sSubPr>
+                                            <m:ctrlPr>
+                                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                            </m:ctrlPr>
+                                          </m:sSubPr>
+                                          <m:e>
+                                            <m:r>
+                                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝑅</m:t>
+                                            </m:r>
+                                          </m:e>
+                                          <m:sub>
+                                            <m:r>
+                                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝐴</m:t>
+                                            </m:r>
+                                          </m:sub>
+                                        </m:sSub>
+                                      </m:num>
+                                      <m:den>
+                                        <m:sSub>
+                                          <m:sSubPr>
+                                            <m:ctrlPr>
+                                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                            </m:ctrlPr>
+                                          </m:sSubPr>
+                                          <m:e>
+                                            <m:r>
+                                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝑅</m:t>
+                                            </m:r>
+                                          </m:e>
+                                          <m:sub>
+                                            <m:r>
+                                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝑝</m:t>
+                                            </m:r>
+                                          </m:sub>
+                                        </m:sSub>
+                                      </m:den>
+                                    </m:f>
+                                  </m:e>
+                                </m:d>
+                              </m:e>
+                            </m:func>
+                          </m:e>
+                        </m:d>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCF1D1E4-28D9-C2D7-1FB8-2754356A24DB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10490199" y="785284"/>
+              <a:ext cx="1758815" cy="502958"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑛_𝑒^longi=(4</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜖_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0 𝑉_𝐴)/(𝑒𝑅_𝑝^2 (1+2 ln⁡(𝑅_𝐴/𝑅_𝑝 ) ) )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>503767</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="862416" cy="367408"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34EDDFF1-A672-86ED-C31E-A8ABC8DEDEC1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9495367" y="821267"/>
+              <a:ext cx="862416" cy="367408"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑛</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>trans</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                    <m:r>
+                      <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜖</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>0</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSubSup>
+                          <m:sSubSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑧</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSubSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑚</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-GB" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑒</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34EDDFF1-A672-86ED-C31E-A8ABC8DEDEC1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9495367" y="821267"/>
+              <a:ext cx="862416" cy="367408"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑛_𝑒^trans=(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜖_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0 𝐵_𝑧^2)/(2𝑚_𝑒 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -2474,10 +3934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16:N17"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2485,41 +3945,42 @@
     <col min="1" max="1" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="51"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="52" t="s">
+      <c r="A2" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="58" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="69"/>
     </row>
-    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -2528,14 +3989,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="21" t="s">
-        <v>16</v>
+      <c r="D3" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="E3" s="22">
-        <v>1000000000000000</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>17</v>
+        <v>0.2</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>45</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>4</v>
@@ -2546,9 +4007,10 @@
       <c r="I3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="24" t="s">
-        <v>30</v>
-      </c>
+      <c r="K3" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2561,20 +4023,20 @@
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>24</v>
+      <c r="D4" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="53">
+        <v>65000</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>46</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="9">
-        <f>B11+H3</f>
+        <f>B12+H3</f>
         <v>958.27208815999995</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -2591,12 +4053,20 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="D5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.06</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>24</v>
+      </c>
       <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="9">
-        <f>SQRT(H4^2 -B11^ 2)</f>
+        <f>SQRT(H4^2 -B12^ 2)</f>
         <v>194.75852619692921</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -2605,49 +4075,50 @@
     </row>
     <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="B6" s="12">
-        <v>1.6726219E-27</v>
+        <v>9.1093837015000008E-31</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="13">
-        <f>(B3*B5^2/2/B7)/(H7^2*B8^2*H8*B6)*E3</f>
-        <v>0.22857438187310988</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
+      <c r="D6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>24</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H6">
-        <f>H5/B11</f>
+        <f>H5/B12</f>
         <v>0.20757148022900346</v>
       </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>11</v>
+      <c r="A7" s="8" t="s">
+        <v>1</v>
       </c>
       <c r="B7" s="12">
-        <v>8.8541878128000006E-12</v>
+        <v>1.6726219E-27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="14">
-        <f>(B3*B5^2/2/B7)*(B11*H8/H5^2*B16)*E3</f>
-        <v>0.22857437861896687</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>15</v>
@@ -2660,47 +4131,44 @@
     </row>
     <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="16">
-        <v>299792458</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="12">
+        <v>8.8541878128000006E-12</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="65">
-        <f>B3*B13^2*H8*B11/(2*B14*H5^2)*E3*B17</f>
-        <v>5870223104.7908945</v>
-      </c>
-      <c r="F8" s="15"/>
+        <v>13</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H8">
-        <f>H4/B11</f>
+        <f>H4/B12</f>
         <v>1.0213157784957891</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="67">
-        <v>197.3269804</v>
+    <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15">
+        <v>299792458</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="9">
-        <f>1/(E6*E4)</f>
-        <v>8.7498869453807568</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="12">
+        <f>(B8*E3^2)/(2*B6)</f>
+        <v>1.9439707674937491E+17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>2</v>
@@ -2710,341 +4178,434 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="26" t="s">
-        <v>32</v>
+    <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="48">
+        <v>197.3269804</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="E10">
-        <f>SQRT(E6)</f>
-        <v>0.4780945323606095</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>33</v>
+        <f>(4*B8*E4)/(B5*E6^2*(1+2*LN(E5/E6)))</f>
+        <v>4211653050641471.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="64">
-        <v>938.27208815999995</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
+    <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="12">
+        <f>MIN(E9:E10)</f>
+        <v>4211653050641471.5</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>938.27208815999995</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="61">
+      <c r="B13" s="44">
         <v>7.2973525693000004E-3</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="13">
+        <f>(B3*B5^2/2/B8)/(H7^2*B9^2*H8*B7)*E11</f>
+        <v>0.96267599271437188</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:15" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <f>SQRT(4*PI()*B12)</f>
+      <c r="B14">
+        <f>SQRT(4*PI()*B13)</f>
         <v>0.30282212087208876</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="E13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="2">
-        <f>SIN(E10*E4)</f>
-        <v>0.23677709214660606</v>
-      </c>
+      <c r="C14" s="4"/>
+      <c r="E14" s="14">
+        <f>(B3*B5^2/2/B8)*(B12*H8/H5^2*B17)*E11</f>
+        <v>0.96267597900905066</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="12"/>
     </row>
-    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="64">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="E14" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="6">
-        <f>COS(E10*E4)</f>
-        <v>0.97156400130644904</v>
-      </c>
-      <c r="I14">
-        <f>1/137</f>
-        <v>7.2992700729927005E-3</v>
-      </c>
-      <c r="J14" s="12">
-        <f>B12-I14</f>
-        <v>-1.9175036927001135E-6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="68">
-        <v>1</v>
-      </c>
       <c r="C15" s="4"/>
+      <c r="E15" s="46">
+        <f>B3*B14^2*H8*B12/(2*B15*H5^2)*E11/B18</f>
+        <v>0.96267597879370392</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="9">
+        <f>1/(E13*E7)</f>
+        <v>2.0775422002171031</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="2">
+        <f>SIN(E17*E7)</f>
+        <v>0.47113779737923661</v>
+      </c>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="63">
+      <c r="B17" s="12">
         <v>6241509074000</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="J16" s="12"/>
-      <c r="K16">
+      <c r="C17" s="4"/>
+      <c r="D17" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <f>SQRT(E13)</f>
+        <v>0.9811605336102609</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="6">
+        <f>COS(E17*E7)</f>
+        <v>0.88205962149995365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="19">
+        <f>C23</f>
+        <v>5067730717679.3955</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="45"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="49">
         <v>1</v>
       </c>
-      <c r="L16" t="s">
-        <v>44</v>
-      </c>
-      <c r="M16">
-        <f>1/B9</f>
+      <c r="B20" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="50">
+        <f>1/B10</f>
         <v>5.0677307176793954E-3</v>
       </c>
-      <c r="N16" t="s">
-        <v>45</v>
+      <c r="D20" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="20">
-        <f>1/B9</f>
+    <row r="21" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="51">
+        <v>1E-13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <f>C20</f>
         <v>5.0677307176793954E-3</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="K17" s="12">
-        <v>1E-13</v>
-      </c>
-      <c r="L17" t="s">
-        <v>46</v>
-      </c>
-      <c r="M17">
-        <f>M16</f>
+      <c r="D21" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" s="51">
+        <f>A21/100</f>
+        <v>1.0000000000000001E-15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <f>C21</f>
         <v>5.0677307176793954E-3</v>
       </c>
+      <c r="D22" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
+    <row r="23" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
+        <v>1</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="5">
+        <f>C22*1000000000000000</f>
+        <v>5067730717679.3955</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="42"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="45"/>
+      <c r="B24" s="12"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="D20" s="29">
-        <f>F13/E10</f>
-        <v>0.4952516210079006</v>
-      </c>
-      <c r="E20" s="29">
-        <f>E15</f>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25"/>
+      <c r="C25" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+      <c r="C26" s="26">
+        <f>I17</f>
+        <v>0.88205962149995365</v>
+      </c>
+      <c r="D26" s="27">
+        <f>I16/E17</f>
+        <v>0.48018421169637382</v>
+      </c>
+      <c r="E26" s="27">
         <v>0</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F26" s="28">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21"/>
-      <c r="C21" s="40" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+      <c r="C27" s="29">
+        <f>-E17*I16</f>
+        <v>-0.46226181268057476</v>
+      </c>
+      <c r="D27" s="30">
+        <f>I17</f>
+        <v>0.88205962149995365</v>
+      </c>
+      <c r="E27" s="30">
+        <v>0</v>
+      </c>
+      <c r="F27" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="29">
+        <v>0</v>
+      </c>
+      <c r="D28" s="30">
+        <v>0</v>
+      </c>
+      <c r="E28" s="30">
+        <f>I17</f>
+        <v>0.88205962149995365</v>
+      </c>
+      <c r="F28" s="31">
+        <f>I16/E17</f>
+        <v>0.48018421169637382</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+      <c r="C29" s="32">
+        <v>0</v>
+      </c>
+      <c r="D29" s="33">
+        <v>0</v>
+      </c>
+      <c r="E29" s="33">
+        <f>-E17*I16</f>
+        <v>-0.46226181268057476</v>
+      </c>
+      <c r="F29" s="34">
+        <f>I17</f>
+        <v>0.88205962149995365</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="32">
-        <f>F14</f>
-        <v>0.97156400130644904</v>
-      </c>
-      <c r="E21" s="32">
+      <c r="B31" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="38">
+        <f t="array" ref="E31:E34">MMULT(C26:F29,B31:B34)</f>
+        <v>0.48904823191961422</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="41">
+        <f>B$31*C26+B$32*D26+B$33*E26+B$34*F26</f>
+        <v>0.48904823191961422</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="41">
+        <f>E31-H31</f>
         <v>0</v>
       </c>
-      <c r="F21" s="33">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="39">
+        <v>0.1</v>
+      </c>
+      <c r="E32" s="39">
+        <v>-0.142924944190292</v>
+      </c>
+      <c r="H32" s="42">
+        <f>B$31*C27+B$32*D27+B$33*E27+B$34*F27</f>
+        <v>-0.142924944190292</v>
+      </c>
+      <c r="K32" s="42">
+        <f>E32-H32</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="C22" s="28">
-        <f>F14</f>
-        <v>0.97156400130644904</v>
-      </c>
-      <c r="D22" s="32">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="35"/>
+      <c r="B33" s="39">
+        <v>-0.3</v>
+      </c>
+      <c r="E33" s="39">
+        <v>-0.36065472878926086</v>
+      </c>
+      <c r="H33" s="42">
+        <f>B$31*C28+B$32*D28+B$33*E28+B$34*F28</f>
+        <v>-0.36065472878926086</v>
+      </c>
+      <c r="K33" s="42">
+        <f>E33-H33</f>
         <v>0</v>
       </c>
-      <c r="E22" s="32">
-        <f>F14</f>
-        <v>0.97156400130644904</v>
-      </c>
-      <c r="F22" s="33">
-        <f>F13/E10</f>
-        <v>0.4952516210079006</v>
-      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="C23" s="31">
-        <f>-E10*F13</f>
-        <v>-0.11320183314353657</v>
-      </c>
-      <c r="D23" s="35">
-        <f>-E15</f>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="40">
+        <v>-0.2</v>
+      </c>
+      <c r="E34" s="40">
+        <v>-3.7733380495818342E-2</v>
+      </c>
+      <c r="H34" s="43">
+        <f>B$31*C29+B$32*D29+B$33*E29+B$34*F29</f>
+        <v>-3.7733380495818342E-2</v>
+      </c>
+      <c r="K34" s="43">
+        <f>E34-H34</f>
         <v>0</v>
       </c>
-      <c r="E23" s="35">
-        <f>-E10*F13</f>
-        <v>-0.11320183314353657</v>
-      </c>
-      <c r="F23" s="36">
-        <f>F14</f>
-        <v>0.97156400130644904</v>
-      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="31">
-        <v>0</v>
-      </c>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-      <c r="C25" s="34">
-        <v>0</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="43" t="e">
-        <f t="array" ref="E25:E28">MMULT(C20:F23,B27:B30)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G25" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="46">
-        <f>B$27*C22+B$28*D20+B$29*E20+B$30*F20</f>
-        <v>0.53530716275401458</v>
-      </c>
-      <c r="J25" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="46" t="e">
-        <f>E25-H25</f>
-        <v>#VALUE!</v>
-      </c>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="E26" s="44" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H26" s="47">
-        <f>B$27*C23+B$28*D21+B$29*E21+B$30*F21</f>
-        <v>4.0555483558876629E-2</v>
-      </c>
-      <c r="K26" s="47" t="e">
-        <f>E26-H26</f>
-        <v>#VALUE!</v>
-      </c>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="E27" s="44" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H27" s="47">
-        <f>B$27*C24+B$28*D22+B$29*E22+B$30*F22</f>
-        <v>-0.3905195245935148</v>
-      </c>
-      <c r="K27" s="47" t="e">
-        <f>E27-H27</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B28" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="E28" s="45" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="H28" s="48">
-        <f>B$27*C25+B$28*D23+B$29*E23+B$30*F23</f>
-        <v>-0.16035225031822886</v>
-      </c>
-      <c r="K28" s="48" t="e">
-        <f>E28-H28</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
-      <c r="B29" s="44">
-        <v>-0.3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B30" s="45">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34"/>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
     <mergeCell ref="G2:I2"/>
+    <mergeCell ref="C25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Partial update to Gabor lens code
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/GaborLens.xlsx
+++ b/21-Spreads4Tests/GaborLens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16619366-3F9E-FB4A-A9B7-F2C75E64207E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44D4B78-B369-EE4F-AE0F-9398E7F2850C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
@@ -1186,15 +1186,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1232,6 +1223,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3937,7 +3937,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3951,34 +3951,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="57"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="61" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="67" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -4007,10 +4007,10 @@
       <c r="I3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="57"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -4203,11 +4203,11 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="66"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="16" t="s">
         <v>16</v>
       </c>
@@ -4428,12 +4428,12 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25"/>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="56"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="69"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26"/>
@@ -4599,13 +4599,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C25:F25"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="G2:I2"/>
-    <mergeCell ref="C25:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Gabor lens update done
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/GaborLens.xlsx
+++ b/21-Spreads4Tests/GaborLens.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44D4B78-B369-EE4F-AE0F-9398E7F2850C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D89B83-48A0-BB42-A33B-F85824FF4BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="34820" yWindow="0" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1186,6 +1186,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1223,15 +1232,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3937,7 +3937,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="E31" sqref="E31:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3951,34 +3951,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="58" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="64" t="s">
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -4007,10 +4007,10 @@
       <c r="I3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="54"/>
+      <c r="L3" s="57"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -4203,11 +4203,11 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="16" t="s">
         <v>16</v>
       </c>
@@ -4428,12 +4428,12 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25"/>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="68"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="69"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="56"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26"/>

</xml_diff>

<commit_message>
Fix transport option for Gabir lens for LhARA
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/GaborLens.xlsx
+++ b/21-Spreads4Tests/GaborLens.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D89B83-48A0-BB42-A33B-F85824FF4BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69A98C2-4458-6747-8EA4-A5A5357BE06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34820" yWindow="0" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>MeV</t>
   </si>
@@ -606,6 +606,60 @@
   </si>
   <si>
     <t>B/l element i/p parameters</t>
+  </si>
+  <si>
+    <t>Solenoid equivalent</t>
+  </si>
+  <si>
+    <r>
+      <t>Strength (B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>m-3</t>
+  </si>
+  <si>
+    <t>ks</t>
+  </si>
+  <si>
+    <t>rad/m</t>
+  </si>
+  <si>
+    <t>1/c</t>
+  </si>
+  <si>
+    <t>s/m</t>
+  </si>
+  <si>
+    <t>1/c*10^9</t>
+  </si>
+  <si>
+    <t>Brho</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -617,7 +671,7 @@
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -704,6 +758,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1095,7 +1165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1186,6 +1256,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,6 +1319,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3934,10 +4020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E34"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3950,37 +4036,51 @@
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67"/>
+      <c r="O1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="60"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="61" t="s">
+      <c r="B2" s="68"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="67" t="s">
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="O2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="55">
+        <v>1.4</v>
+      </c>
+      <c r="Q2" s="56" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
@@ -4007,12 +4107,14 @@
       <c r="I3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="57" t="s">
+      <c r="K3" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="57"/>
+      <c r="L3" s="64"/>
+      <c r="O3" s="57"/>
+      <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -4042,8 +4144,18 @@
       <c r="I4" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="O4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" s="19">
+        <f>B8/(2*B7*H8)*P2^2</f>
+        <v>5079453457989577</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
@@ -4073,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>52</v>
       </c>
@@ -4100,8 +4212,17 @@
         <v>0.20757148022900346</v>
       </c>
       <c r="I6" s="4"/>
+      <c r="O6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="77">
+        <v>2.491695</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>1</v>
       </c>
@@ -4128,8 +4249,15 @@
         <v>0.20323927682260837</v>
       </c>
       <c r="I7" s="4"/>
+      <c r="O7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7">
+        <f>2*P16*P6</f>
+        <v>3.2374319832439378</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -4150,7 +4278,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
@@ -4178,7 +4306,7 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>39</v>
       </c>
@@ -4201,13 +4329,22 @@
       <c r="G10" s="11"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
+      <c r="O10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="50">
+        <v>299792458</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+    <row r="11" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="66"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="73"/>
       <c r="D11" s="16" t="s">
         <v>16</v>
       </c>
@@ -4222,9 +4359,18 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
+      <c r="O11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11">
+        <f>1/P10</f>
+        <v>3.3356409519815204E-9</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -4235,8 +4381,18 @@
         <v>0</v>
       </c>
       <c r="F12" s="4"/>
+      <c r="O12" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="P12" s="5">
+        <f>P11*1000000000</f>
+        <v>3.3356409519815204</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" ht="19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
@@ -4255,7 +4411,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
@@ -4273,7 +4429,7 @@
       </c>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
@@ -4290,7 +4446,7 @@
       </c>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="47" t="s">
         <v>39</v>
       </c>
@@ -4316,8 +4472,15 @@
         <v>0.47113779737923661</v>
       </c>
       <c r="J16" s="12"/>
+      <c r="O16" t="s">
+        <v>65</v>
+      </c>
+      <c r="P16">
+        <f>H5*P12/1000</f>
+        <v>0.64964451573004278</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>25</v>
       </c>
@@ -4342,8 +4505,15 @@
         <f>COS(E17*E7)</f>
         <v>0.88205962149995365</v>
       </c>
+      <c r="O17" t="s">
+        <v>60</v>
+      </c>
+      <c r="P17">
+        <f>P2/(2*P16)</f>
+        <v>1.0775123672265128</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>38</v>
       </c>
@@ -4357,11 +4527,18 @@
       <c r="F18" s="6"/>
       <c r="H18" s="16"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="45"/>
       <c r="B19" s="12"/>
+      <c r="O19" t="s">
+        <v>66</v>
+      </c>
+      <c r="P19">
+        <f>2*P16*P17</f>
+        <v>1.4</v>
+      </c>
     </row>
-    <row r="20" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="49">
         <v>1</v>
       </c>
@@ -4376,7 +4553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="51">
         <v>1E-13</v>
       </c>
@@ -4391,7 +4568,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="51">
         <f>A21/100</f>
         <v>1.0000000000000001E-15</v>
@@ -4407,7 +4584,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>1</v>
       </c>
@@ -4422,20 +4599,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="45"/>
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25"/>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="56"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="63"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="C26" s="26">
         <f>I17</f>
@@ -4452,7 +4629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="C27" s="29">
         <f>-E17*I16</f>
@@ -4469,7 +4646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="36"/>
       <c r="B28" s="37"/>
       <c r="C28" s="29">
@@ -4487,7 +4664,7 @@
         <v>0.48018421169637382</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="C29" s="32">
         <v>0</v>
@@ -4504,10 +4681,10 @@
         <v>0.88205962149995365</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
         <v>36</v>
       </c>
@@ -4536,7 +4713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B32" s="39">
         <v>0.1</v>
       </c>
@@ -4598,7 +4775,8 @@
       <c r="A41"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="O1:Q1"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="A1:I1"/>

</xml_diff>